<commit_message>
Ticket 002: nice header and background created for both pages
</commit_message>
<xml_diff>
--- a/User Stories.xlsx
+++ b/User Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zsigm\Desktop\homework\rick-and-morty-catalog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DC7998F-6EE0-465F-8EDF-9C718CBE37C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07509B4E-8A60-4043-BF3B-FD4180F01F7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>Task</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>https://github.com/zsigmondO/rick-and-morty-catalog/pull/1</t>
   </si>
 </sst>
 </file>
@@ -253,7 +256,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -265,26 +268,23 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -569,24 +569,24 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.88671875" customWidth="1"/>
     <col min="4" max="4" width="30.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -606,10 +606,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="10">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -621,15 +621,18 @@
       <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -641,22 +644,25 @@
       <c r="E3" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="G3" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -669,11 +675,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
+    <row r="6" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
         <v>4</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -686,14 +692,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
+    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -703,11 +709,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
+    <row r="8" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
         <v>6</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -720,11 +726,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
+    <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -738,19 +744,19 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5">
         <v>8</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -764,10 +770,10 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>9</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>36</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -781,10 +787,10 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>10</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -798,19 +804,19 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>11</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -824,10 +830,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="6">
+      <c r="A16" s="5">
         <v>12</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -841,22 +847,22 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>

</xml_diff>